<commit_message>
[Parking] Update Parking Schedule
</commit_message>
<xml_diff>
--- a/APP/Parking/doc/PIS/Schedule_Parking.xlsx
+++ b/APP/Parking/doc/PIS/Schedule_Parking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="0" windowWidth="26920" windowHeight="18180" tabRatio="500"/>
+    <workbookView xWindow="2180" yWindow="20" windowWidth="31480" windowHeight="19980" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Item Schedule" sheetId="3" r:id="rId1"/>
@@ -252,14 +252,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>scrollDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>change func</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>manday, 人天</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -889,10 +881,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>27.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>1. change func               2.getSiteData():</t>
     </r>
@@ -911,6 +899,130 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">1. on("click") func           2. getSpaceData()         3.getAPIListAllParkingSpace() : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>index.js</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.getAPIListAllTime(): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>index.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                       2. getParkingStatus() -&gt;grepData: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">index.js </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">      3. getReserveData()      4.getAPIQueryReserveDetail()                             5. on("click") func         6.getAPIQueryMyReserveTime()</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. getReserveBtn()       2.reserveBtnDefaultStatus()                               3. on("click") func -&gt; QTY  點選下一步跳到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">頁面 2.1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4.getAPIReserveParkingSpace()</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. delete click                 2. querySettingList()      3. button on("click") func -&gt;跳到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>頁面 3.1</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.getAPIQueryMyReserve()  2.getAPIMyReserveCancel()                                 3. on("click") func         4. cancel click</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. setDefaultStatus()     2. changeEditStatus()      3. save click                 4. delete click              5. back click </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scrollDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">1. on("click") func             2. setRole()                   3. setDateList()              4. getAPIListAllManager(): </t>
     </r>
     <r>
@@ -949,123 +1061,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. on("click") func           2. getSpaceData()         3.getAPIListAllParkingSpace() : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>index.js</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1.getAPIListAllTime(): </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>index.js</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                       2. getParkingStatus() -&gt;grepData: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">index.js </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">      3. getReserveData()      4.getAPIQueryReserveDetail()                             5. on("click") func         6.getAPIQueryMyReserveTime()</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. getReserveBtn()       2.reserveBtnDefaultStatus()                               3. on("click") func -&gt; QTY  點選下一步跳到</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">頁面 2.1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4.getAPIReserveParkingSpace()</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. delete click                 2. querySettingList()      3. button on("click") func -&gt;跳到</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>頁面 3.1</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.getAPIQueryMyReserve()  2.getAPIMyReserveCancel()                                 3. on("click") func         4. cancel click</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1. setDefaultStatus()     2. changeEditStatus()      3. save click                 4. delete click              5. back click </t>
+    <t xml:space="preserve">1. change func                2. APP_common.js </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>29.3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1430,7 +1430,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1503,11 +1503,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="63">
@@ -1904,8 +1907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1919,18 +1922,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="A1" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="9"/>
@@ -1962,7 +1965,7 @@
         <v>27</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>28</v>
@@ -1976,7 +1979,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -1988,7 +1991,7 @@
       <c r="I4" s="15"/>
       <c r="J4" s="16"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" ht="33" customHeight="1">
       <c r="A5" s="17" t="s">
         <v>35</v>
       </c>
@@ -1999,16 +2002,16 @@
         <v>47</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>50</v>
+        <v>181</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>42</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="26">
-        <v>0.1</v>
+        <v>51</v>
+      </c>
+      <c r="G5" s="32">
+        <v>2</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>31</v>
@@ -2025,25 +2028,25 @@
     </row>
     <row r="7" spans="1:10" ht="30">
       <c r="A7" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>41</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="26">
-        <v>0.5</v>
+        <v>52</v>
+      </c>
+      <c r="G7" s="32">
+        <v>0.8</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>32</v>
@@ -2051,22 +2054,22 @@
     </row>
     <row r="8" spans="1:10" ht="128" customHeight="1">
       <c r="A8" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>48</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>49</v>
+        <v>179</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G8" s="26">
         <v>2</v>
@@ -2079,22 +2082,22 @@
     </row>
     <row r="9" spans="1:10" ht="65" customHeight="1">
       <c r="A9" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>39</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G9" s="26">
         <v>2</v>
@@ -2105,84 +2108,84 @@
       <c r="I9" s="12"/>
       <c r="J9" s="13"/>
     </row>
-    <row r="10" spans="1:10" ht="125" customHeight="1">
+    <row r="10" spans="1:10" ht="150">
       <c r="A10" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>71</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="G10" s="26">
         <v>5</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I10" s="12"/>
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" ht="129" customHeight="1">
       <c r="A11" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G11" s="26">
         <v>2</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I11" s="12"/>
       <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10" ht="43" customHeight="1">
       <c r="A12" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>131</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>133</v>
       </c>
       <c r="G12" s="26">
         <v>1</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I12" s="12"/>
       <c r="J12" s="13"/>
@@ -2194,7 +2197,7 @@
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="12"/>
@@ -2205,35 +2208,35 @@
     </row>
     <row r="14" spans="1:10" ht="64" customHeight="1">
       <c r="A14" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B14" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>138</v>
-      </c>
       <c r="D14" s="15" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G14" s="26">
         <v>2.5</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I14" s="12"/>
       <c r="J14" s="13"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -2247,35 +2250,35 @@
     </row>
     <row r="16" spans="1:10" ht="91" customHeight="1">
       <c r="A16" s="17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B16" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F16" s="12" t="s">
         <v>125</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>127</v>
       </c>
       <c r="G16" s="26">
         <v>3</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I16" s="12"/>
       <c r="J16" s="13"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -2289,7 +2292,7 @@
     </row>
     <row r="18" spans="1:10" ht="37" customHeight="1">
       <c r="A18" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -2303,59 +2306,59 @@
     </row>
     <row r="19" spans="1:10" ht="187" customHeight="1">
       <c r="A19" s="17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G19" s="26">
         <v>4</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I19" s="12"/>
       <c r="J19" s="13"/>
     </row>
     <row r="20" spans="1:10" ht="80" customHeight="1">
       <c r="A20" s="17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G20" s="26">
         <v>2</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I20" s="12"/>
       <c r="J20" s="13"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -2372,38 +2375,38 @@
         <v>3.1</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G22" s="26">
         <v>3</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I22" s="12"/>
       <c r="J22" s="13"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="12"/>
-      <c r="G23" s="31" t="s">
-        <v>174</v>
+      <c r="G23" s="30" t="s">
+        <v>182</v>
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -2548,8 +2551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L49"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2568,7 +2571,7 @@
   <sheetData>
     <row r="3" spans="2:12">
       <c r="F3" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H3" s="5"/>
     </row>
@@ -2578,13 +2581,13 @@
     <row r="5" spans="2:12">
       <c r="B5" s="2"/>
       <c r="C5" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -2592,41 +2595,41 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="2:12">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="H6" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="2:12">
@@ -2640,7 +2643,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>16</v>
@@ -2652,13 +2655,13 @@
         <v>18</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>18</v>
@@ -2697,10 +2700,10 @@
     <row r="10" spans="2:12">
       <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>10</v>
@@ -2715,10 +2718,10 @@
         <v>24</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>7</v>
@@ -2760,7 +2763,7 @@
     <row r="13" spans="2:12">
       <c r="B13" s="3"/>
       <c r="C13" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
@@ -2778,10 +2781,10 @@
         <v>24</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>8</v>
@@ -2811,13 +2814,13 @@
         <v>25</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>8</v>
@@ -2856,7 +2859,7 @@
     <row r="17" spans="2:12">
       <c r="B17" s="3"/>
       <c r="C17" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>11</v>
@@ -2871,16 +2874,16 @@
         <v>21</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>7</v>
@@ -2889,10 +2892,10 @@
     <row r="18" spans="2:12">
       <c r="B18" s="3"/>
       <c r="C18" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>12</v>
@@ -2904,16 +2907,16 @@
         <v>22</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>8</v>
@@ -2922,7 +2925,7 @@
     <row r="19" spans="2:12">
       <c r="B19" s="3"/>
       <c r="C19" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>7</v>
@@ -2937,16 +2940,16 @@
         <v>22</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>7</v>
@@ -2955,10 +2958,10 @@
     <row r="20" spans="2:12">
       <c r="B20" s="3"/>
       <c r="C20" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>13</v>
@@ -2973,13 +2976,13 @@
         <v>24</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>8</v>
@@ -3003,10 +3006,10 @@
         <v>5</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>8</v>
@@ -3021,16 +3024,16 @@
         <v>8</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="2:12">
@@ -3066,13 +3069,13 @@
     <row r="25" spans="2:12">
       <c r="B25" s="3"/>
       <c r="C25" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D25" s="29">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="E25" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="F25" s="1">
         <v>2</v>
@@ -3116,17 +3119,17 @@
     <row r="28" spans="2:12">
       <c r="B28" s="2"/>
       <c r="C28" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D28" s="27">
         <v>2.1</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
@@ -3136,14 +3139,14 @@
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
@@ -3157,7 +3160,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -3197,13 +3200,13 @@
     <row r="33" spans="2:10">
       <c r="B33" s="3"/>
       <c r="C33" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1" t="s">
@@ -3242,13 +3245,13 @@
     <row r="36" spans="2:10">
       <c r="B36" s="3"/>
       <c r="C36" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
@@ -3264,10 +3267,10 @@
         <v>3</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
@@ -3306,13 +3309,13 @@
     <row r="40" spans="2:10">
       <c r="B40" s="3"/>
       <c r="C40" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
@@ -3325,13 +3328,13 @@
     <row r="41" spans="2:10">
       <c r="B41" s="3"/>
       <c r="C41" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
@@ -3344,13 +3347,13 @@
     <row r="42" spans="2:10">
       <c r="B42" s="3"/>
       <c r="C42" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
@@ -3363,13 +3366,13 @@
     <row r="43" spans="2:10">
       <c r="B43" s="3"/>
       <c r="C43" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
@@ -3395,13 +3398,13 @@
         <v>5</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1" t="s">
@@ -3440,7 +3443,7 @@
     <row r="48" spans="2:10">
       <c r="B48" s="3"/>
       <c r="C48" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D48" s="29">
         <v>4</v>

</xml_diff>